<commit_message>
Working Exponential Lockout, Data now protected SQL side
</commit_message>
<xml_diff>
--- a/rawData/attic.xlsx
+++ b/rawData/attic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brack\Documents\Peter Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brack\Documents\GitHub\filmDatabase\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8058797A-F88D-4652-A0F4-CD47C37F00B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0045B6E-2677-4CAE-ADCE-15C9259035AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8079E1E-8BBE-4E12-8DA2-CB5E3D9690F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="203">
   <si>
     <t>name</t>
   </si>
@@ -645,9 +645,6 @@
   </si>
   <si>
     <t>Reservoir Dogs</t>
-  </si>
-  <si>
-    <t>BLANK (PG) if film</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41851449-5515-4382-A245-82EA6364A766}">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="H180" sqref="H180"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1713,7 +1710,7 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>